<commit_message>
dataram added, wait for debug
</commit_message>
<xml_diff>
--- a/Report 22.6 成型多周期 CPU/59 全部指令集完全版分析.xlsx
+++ b/Report 22.6 成型多周期 CPU/59 全部指令集完全版分析.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VIVADO_project\Disjunctive.N.F\Report 22.6 成型多周期 CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EA9713-A34F-461F-A37B-E8B615A62202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B4DF7A-80F3-4C86-83EE-9CAA17719DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1874" uniqueCount="295">
   <si>
     <t>opcode</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1393,13 +1393,10 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1408,16 +1405,19 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1702,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AP6" sqref="AP6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q71" sqref="Q71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1825,10 +1825,10 @@
       </c>
     </row>
     <row r="3" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="22" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1873,19 +1873,19 @@
       </c>
     </row>
     <row r="4" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="1" t="s">
         <v>177</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
       <c r="N4" s="13" t="s">
         <v>207</v>
       </c>
@@ -1900,15 +1900,15 @@
       </c>
     </row>
     <row r="5" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
       <c r="N5" s="14" t="s">
         <v>209</v>
       </c>
@@ -1917,14 +1917,14 @@
       </c>
     </row>
     <row r="6" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29" t="s">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1936,8 +1936,8 @@
       </c>
     </row>
     <row r="7" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="1" t="s">
         <v>163</v>
       </c>
@@ -2079,57 +2079,57 @@
       <c r="BK15" s="14"/>
     </row>
     <row r="16" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="I16" s="24">
+      <c r="I16" s="26">
         <v>2</v>
       </c>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24">
+      <c r="J16" s="26"/>
+      <c r="K16" s="26">
         <v>3</v>
       </c>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24">
+      <c r="L16" s="26"/>
+      <c r="M16" s="26">
         <v>13</v>
       </c>
-      <c r="N16" s="24"/>
+      <c r="N16" s="26"/>
       <c r="O16" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="P16" s="24">
+      <c r="P16" s="26">
         <v>4</v>
       </c>
-      <c r="Q16" s="24"/>
+      <c r="Q16" s="26"/>
       <c r="R16" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="S16" s="24">
+      <c r="S16" s="26">
         <v>3</v>
       </c>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24">
+      <c r="T16" s="26"/>
+      <c r="U16" s="26">
         <v>2</v>
       </c>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24">
+      <c r="V16" s="26"/>
+      <c r="W16" s="26">
         <v>2</v>
       </c>
-      <c r="X16" s="24"/>
+      <c r="X16" s="26"/>
       <c r="Y16" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="Z16" s="24">
+      <c r="Z16" s="26">
         <v>2</v>
       </c>
-      <c r="AA16" s="24"/>
+      <c r="AA16" s="26"/>
       <c r="AB16" s="4" t="s">
         <v>290</v>
       </c>
       <c r="AC16" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="AD16" s="24">
+      <c r="AD16" s="26">
         <v>4</v>
       </c>
-      <c r="AE16" s="24"/>
+      <c r="AE16" s="26"/>
       <c r="AF16" s="4" t="s">
         <v>290</v>
       </c>
@@ -2170,14 +2170,14 @@
     <row r="17" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
       <c r="I17" s="27" t="s">
         <v>186</v>
       </c>
@@ -2200,35 +2200,35 @@
       <c r="R17" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="S17" s="25" t="s">
+      <c r="S17" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="T17" s="26"/>
-      <c r="U17" s="25" t="s">
+      <c r="T17" s="25"/>
+      <c r="U17" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="V17" s="26"/>
-      <c r="W17" s="22" t="s">
+      <c r="V17" s="25"/>
+      <c r="W17" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="X17" s="23"/>
+      <c r="X17" s="30"/>
       <c r="Y17" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="Z17" s="22" t="s">
+      <c r="Z17" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="AA17" s="23"/>
+      <c r="AA17" s="30"/>
       <c r="AB17" s="16" t="s">
         <v>244</v>
       </c>
       <c r="AC17" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="AD17" s="25" t="s">
+      <c r="AD17" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="AE17" s="26"/>
+      <c r="AE17" s="25"/>
       <c r="AF17" s="20" t="s">
         <v>251</v>
       </c>
@@ -8280,9 +8280,11 @@
       <c r="O66" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="P66" s="10"/>
+      <c r="P66" s="10" t="s">
+        <v>225</v>
+      </c>
       <c r="Q66" s="2" t="s">
-        <v>107</v>
+        <v>270</v>
       </c>
       <c r="R66" s="6" t="s">
         <v>106</v>
@@ -8407,9 +8409,11 @@
       <c r="O67" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="P67" s="10"/>
+      <c r="P67" s="10" t="s">
+        <v>225</v>
+      </c>
       <c r="Q67" s="2" t="s">
-        <v>107</v>
+        <v>270</v>
       </c>
       <c r="R67" s="6" t="s">
         <v>106</v>
@@ -8534,9 +8538,11 @@
       <c r="O68" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="P68" s="10"/>
+      <c r="P68" s="10" t="s">
+        <v>225</v>
+      </c>
       <c r="Q68" s="2" t="s">
-        <v>107</v>
+        <v>269</v>
       </c>
       <c r="R68" s="6" t="s">
         <v>106</v>
@@ -8661,9 +8667,11 @@
       <c r="O69" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="P69" s="10"/>
+      <c r="P69" s="10" t="s">
+        <v>225</v>
+      </c>
       <c r="Q69" s="2" t="s">
-        <v>107</v>
+        <v>269</v>
       </c>
       <c r="R69" s="6" t="s">
         <v>106</v>
@@ -8788,9 +8796,11 @@
       <c r="O70" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="P70" s="10"/>
+      <c r="P70" s="10" t="s">
+        <v>225</v>
+      </c>
       <c r="Q70" s="2" t="s">
-        <v>107</v>
+        <v>269</v>
       </c>
       <c r="R70" s="6" t="s">
         <v>106</v>
@@ -8915,9 +8925,11 @@
       <c r="O71" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="P71" s="10"/>
+      <c r="P71" s="10" t="s">
+        <v>225</v>
+      </c>
       <c r="Q71" s="2" t="s">
-        <v>107</v>
+        <v>269</v>
       </c>
       <c r="R71" s="6" t="s">
         <v>204</v>
@@ -9038,9 +9050,11 @@
       <c r="O72" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="P72" s="10"/>
+      <c r="P72" s="10" t="s">
+        <v>225</v>
+      </c>
       <c r="Q72" s="2" t="s">
-        <v>107</v>
+        <v>269</v>
       </c>
       <c r="R72" s="6" t="s">
         <v>204</v>
@@ -9161,9 +9175,11 @@
       <c r="O73" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="P73" s="10"/>
+      <c r="P73" s="10" t="s">
+        <v>225</v>
+      </c>
       <c r="Q73" s="2" t="s">
-        <v>107</v>
+        <v>269</v>
       </c>
       <c r="R73" s="6" t="s">
         <v>204</v>
@@ -10157,12 +10173,12 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="W16:X16"/>
+    <mergeCell ref="Z16:AA16"/>
+    <mergeCell ref="Z17:AA17"/>
+    <mergeCell ref="AD17:AE17"/>
+    <mergeCell ref="AD16:AE16"/>
     <mergeCell ref="U17:V17"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="K16:L16"/>
@@ -10175,12 +10191,12 @@
     <mergeCell ref="M17:N17"/>
     <mergeCell ref="P17:Q17"/>
     <mergeCell ref="S17:T17"/>
-    <mergeCell ref="W17:X17"/>
-    <mergeCell ref="W16:X16"/>
-    <mergeCell ref="Z16:AA16"/>
-    <mergeCell ref="Z17:AA17"/>
-    <mergeCell ref="AD17:AE17"/>
-    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="D5:H5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>